<commit_message>
Building in supply side
</commit_message>
<xml_diff>
--- a/results/08-2023/comparison-deflators-08-2023.xlsx
+++ b/results/08-2023/comparison-deflators-08-2023.xlsx
@@ -1449,43 +1449,43 @@
         <v>-4.8299</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.5026</v>
+        <v>-2.4186</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.9763</v>
+        <v>-0.9767</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.0816</v>
+        <v>0.0753</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.7839</v>
+        <v>-0.3713</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.376</v>
+        <v>-0.0351</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.2835</v>
+        <v>0.2572</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.5339</v>
+        <v>0.0139</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.0419</v>
+        <v>0.9707</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.062</v>
+        <v>0.0487</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0595</v>
+        <v>0.0594</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.0679</v>
+        <v>-0.323</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.12</v>
+        <v>-0.6118</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0823</v>
+        <v>0.072</v>
       </c>
     </row>
     <row r="17">
@@ -3185,43 +3185,43 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0022</v>
+        <v>0.0862</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.0766</v>
+        <v>-0.077</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.0743</v>
+        <v>0.0826</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.0437</v>
+        <v>0.369</v>
       </c>
       <c r="L44" t="n">
-        <v>-0.0715</v>
+        <v>0.2694</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0091</v>
+        <v>0.5498</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0139</v>
+        <v>0.5617</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.0244</v>
+        <v>0.9883</v>
       </c>
       <c r="P44" t="n">
-        <v>0.0044</v>
+        <v>0.1151</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.0018</v>
+        <v>0.0016</v>
       </c>
       <c r="R44" t="n">
-        <v>0.0043</v>
+        <v>-0.2508</v>
       </c>
       <c r="S44" t="n">
-        <v>72.5899</v>
+        <v>72.098</v>
       </c>
       <c r="T44" t="n">
-        <v>1.967</v>
+        <v>1.9566</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
Supply side 2nd revisions plus preparation of forecast sheet
</commit_message>
<xml_diff>
--- a/results/08-2023/comparison-deflators-08-2023.xlsx
+++ b/results/08-2023/comparison-deflators-08-2023.xlsx
@@ -1449,43 +1449,43 @@
         <v>-4.8299</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.4186</v>
+        <v>-2.2786</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.9767</v>
+        <v>-0.9468</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0753</v>
+        <v>0.3035</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.3713</v>
+        <v>-0.2685</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.0351</v>
+        <v>0.1537</v>
       </c>
       <c r="M16" t="n">
-        <v>0.2572</v>
+        <v>0.0528</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0139</v>
+        <v>-0.3846</v>
       </c>
       <c r="O16" t="n">
-        <v>0.9707</v>
+        <v>-0.094</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0487</v>
+        <v>-0.2777</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0594</v>
+        <v>-0.1541</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.323</v>
+        <v>-0.7807</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.6118</v>
+        <v>-0.5667</v>
       </c>
       <c r="T16" t="n">
-        <v>0.072</v>
+        <v>0.0906</v>
       </c>
     </row>
     <row r="17">
@@ -3185,43 +3185,43 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0862</v>
+        <v>0.2262</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.077</v>
+        <v>-0.0471</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0826</v>
+        <v>0.3108</v>
       </c>
       <c r="K44" t="n">
-        <v>0.369</v>
+        <v>0.4717</v>
       </c>
       <c r="L44" t="n">
-        <v>0.2694</v>
+        <v>0.4582</v>
       </c>
       <c r="M44" t="n">
-        <v>0.5498</v>
+        <v>0.3454</v>
       </c>
       <c r="N44" t="n">
-        <v>0.5617</v>
+        <v>0.1632</v>
       </c>
       <c r="O44" t="n">
-        <v>0.9883</v>
+        <v>-0.0765</v>
       </c>
       <c r="P44" t="n">
-        <v>0.1151</v>
+        <v>-0.2112</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.0016</v>
+        <v>-0.2118</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.2508</v>
+        <v>-0.7086</v>
       </c>
       <c r="S44" t="n">
-        <v>72.098</v>
+        <v>72.1432</v>
       </c>
       <c r="T44" t="n">
-        <v>1.9566</v>
+        <v>1.9752</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
Fim run Aug 31
</commit_message>
<xml_diff>
--- a/results/08-2023/comparison-deflators-08-2023.xlsx
+++ b/results/08-2023/comparison-deflators-08-2023.xlsx
@@ -590,7 +590,7 @@
         <v>0.0101</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0065</v>
+        <v>0.0062</v>
       </c>
       <c r="L2" t="n">
         <v>0.0074</v>
@@ -729,7 +729,7 @@
         <v>-0.0179</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0682</v>
+        <v>-0.0683</v>
       </c>
       <c r="Q4" t="n">
         <v>-0.0296</v>
@@ -738,10 +738,10 @@
         <v>-0.0286</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.0269</v>
+        <v>-0.027</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.0262</v>
+        <v>-0.0263</v>
       </c>
     </row>
     <row r="5">
@@ -776,34 +776,34 @@
         <v>0.1308</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.2314</v>
+        <v>-0.1969</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1857</v>
+        <v>-0.186</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.1942</v>
+        <v>-0.1945</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.3946</v>
+        <v>-0.3951</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.4932</v>
+        <v>-0.4939</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.1428</v>
+        <v>-0.143</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.1424</v>
+        <v>-0.1426</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.4593</v>
+        <v>-0.46</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.4577</v>
+        <v>-0.4584</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.1226</v>
+        <v>-0.1227</v>
       </c>
     </row>
     <row r="6">
@@ -838,34 +838,34 @@
         <v>-0.0546</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0595</v>
+        <v>-0.0499</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0426</v>
+        <v>-0.0331</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0374</v>
+        <v>-0.028</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0258</v>
+        <v>-0.0166</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.0111</v>
+        <v>-0.0021</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0134</v>
+        <v>-0.0045</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.0026</v>
+        <v>0.0061</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.0066</v>
+        <v>0.0077</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0033</v>
+        <v>0.0232</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0101</v>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="7">
@@ -900,34 +900,34 @@
         <v>-0.04</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0632</v>
+        <v>0.0647</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0264</v>
+        <v>-0.0083</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0047</v>
+        <v>-0.0386</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.0945</v>
+        <v>-0.1277</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.092</v>
+        <v>-0.126</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.0639</v>
+        <v>-0.0625</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0052</v>
+        <v>0.0066</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0699</v>
+        <v>0.0712</v>
       </c>
       <c r="S7" t="n">
-        <v>0.1162</v>
+        <v>0.1177</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1625</v>
+        <v>0.1641</v>
       </c>
     </row>
     <row r="8">
@@ -962,34 +962,34 @@
         <v>0.2526</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3161</v>
+        <v>0.3134</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1783</v>
+        <v>0.1311</v>
       </c>
       <c r="M8" t="n">
-        <v>0.2451</v>
+        <v>0.1561</v>
       </c>
       <c r="N8" t="n">
-        <v>0.5261</v>
+        <v>0.4183</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5233</v>
+        <v>0.3973</v>
       </c>
       <c r="P8" t="n">
-        <v>0.5536</v>
+        <v>0.4102</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4624</v>
+        <v>0.2994</v>
       </c>
       <c r="R8" t="n">
-        <v>0.2485</v>
+        <v>0.0696</v>
       </c>
       <c r="S8" t="n">
-        <v>0.2756</v>
+        <v>0.0846</v>
       </c>
       <c r="T8" t="n">
-        <v>0.2637</v>
+        <v>0.0789</v>
       </c>
     </row>
     <row r="9">
@@ -1086,25 +1086,25 @@
         <v>-0.0899</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0972</v>
+        <v>-0.0971</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.096</v>
+        <v>-0.0961</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.0983</v>
+        <v>-0.0985</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.0632</v>
+        <v>-0.0633</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.0498</v>
+        <v>-0.0499</v>
       </c>
       <c r="P10" t="n">
         <v>-0.0442</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0263</v>
+        <v>-0.0264</v>
       </c>
       <c r="R10" t="n">
         <v>-0.0105</v>
@@ -1148,7 +1148,7 @@
         <v>0.0079</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0065</v>
+        <v>0.0058</v>
       </c>
       <c r="L11" t="n">
         <v>0.0083</v>
@@ -1210,34 +1210,34 @@
         <v>0.0463</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0805</v>
+        <v>0.0841</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1297</v>
+        <v>0.1334</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0755</v>
+        <v>-0.0722</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.1626</v>
+        <v>-0.1594</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0768</v>
+        <v>-0.077</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0708</v>
+        <v>-0.0709</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0376</v>
+        <v>-0.0377</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.074</v>
+        <v>-0.0742</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.0722</v>
+        <v>-0.0723</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0691</v>
+        <v>-0.0693</v>
       </c>
     </row>
     <row r="13">
@@ -1248,58 +1248,58 @@
         <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.0646</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>0.0296</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.0274</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.0173</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>-0.0131</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>-0.0124</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>-0.0118</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>-0.0109</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>-0.0095</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0043</v>
+        <v>-0.1368</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0031</v>
+        <v>-0.1146</v>
       </c>
       <c r="N13" t="n">
-        <v>0.004</v>
+        <v>-0.104</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0022</v>
+        <v>-0.0952</v>
       </c>
       <c r="P13" t="n">
-        <v>0.0021</v>
+        <v>-0.0561</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0018</v>
+        <v>-0.0305</v>
       </c>
       <c r="R13" t="n">
-        <v>0.0017</v>
+        <v>-0.0302</v>
       </c>
       <c r="S13" t="n">
-        <v>0.0017</v>
+        <v>-0.0238</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0017</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="14">
@@ -1337,28 +1337,28 @@
         <v>-0.5068</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.5761</v>
+        <v>-0.5769</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.2263</v>
+        <v>-0.2266</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.1787</v>
+        <v>-0.1789</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.3214</v>
+        <v>-0.3218</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2393</v>
+        <v>-0.2396</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1041</v>
+        <v>-0.1042</v>
       </c>
       <c r="R14" t="n">
         <v>-0.0329</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0262</v>
+        <v>-0.0263</v>
       </c>
       <c r="T14" t="n">
         <v>-0.0193</v>
@@ -1399,10 +1399,10 @@
         <v>-0.2839</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.1293</v>
+        <v>-0.1294</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.0075</v>
+        <v>-0.0076</v>
       </c>
       <c r="N15" t="n">
         <v>-0.0014</v>
@@ -1434,58 +1434,58 @@
         <v>21</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.1407</v>
+        <v>-2.0761</v>
       </c>
       <c r="D16" t="n">
-        <v>-2.525</v>
+        <v>-2.4954</v>
       </c>
       <c r="E16" t="n">
-        <v>-3.1302</v>
+        <v>-3.1028</v>
       </c>
       <c r="F16" t="n">
-        <v>-3.8752</v>
+        <v>-3.8579</v>
       </c>
       <c r="G16" t="n">
-        <v>-4.8299</v>
+        <v>-4.8431</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.2786</v>
+        <v>-2.3359</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.9468</v>
+        <v>-0.9889</v>
       </c>
       <c r="J16" t="n">
-        <v>0.3035</v>
+        <v>0.2775</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.2685</v>
+        <v>-0.2151</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1537</v>
+        <v>-0.1467</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0528</v>
+        <v>-0.1349</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.3846</v>
+        <v>-0.5118</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.094</v>
+        <v>-0.3448</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.2777</v>
+        <v>-0.395</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.1541</v>
+        <v>-0.2597</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.7807</v>
+        <v>-0.4655</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.5667</v>
+        <v>-0.5068</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0906</v>
+        <v>-0.2111</v>
       </c>
     </row>
     <row r="17">
@@ -1520,34 +1520,34 @@
         <v>26529.8</v>
       </c>
       <c r="K17" t="n">
-        <v>26835</v>
+        <v>26798.6</v>
       </c>
       <c r="L17" t="n">
-        <v>27066.6327</v>
+        <v>27029.9185</v>
       </c>
       <c r="M17" t="n">
-        <v>27338.6735</v>
+        <v>27301.5903</v>
       </c>
       <c r="N17" t="n">
-        <v>27651.3265</v>
+        <v>27613.8192</v>
       </c>
       <c r="O17" t="n">
-        <v>27981.7347</v>
+        <v>27943.7792</v>
       </c>
       <c r="P17" t="n">
-        <v>28318.8776</v>
+        <v>28280.4648</v>
       </c>
       <c r="Q17" t="n">
-        <v>28667.9592</v>
+        <v>28629.0729</v>
       </c>
       <c r="R17" t="n">
-        <v>29023.6735</v>
+        <v>28984.3047</v>
       </c>
       <c r="S17" t="n">
-        <v>29370.9184</v>
+        <v>29331.0786</v>
       </c>
       <c r="T17" t="n">
-        <v>29713.2653</v>
+        <v>29672.9611</v>
       </c>
     </row>
     <row r="18">
@@ -1582,31 +1582,31 @@
         <v>-0.141</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.1731</v>
+        <v>-0.1584</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.1349</v>
+        <v>-0.1351</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.0605</v>
+        <v>-0.0606</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.2613</v>
+        <v>-0.2616</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.3741</v>
+        <v>-0.3746</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0169</v>
+        <v>-0.017</v>
       </c>
       <c r="Q18" t="n">
         <v>0.0097</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.3161</v>
+        <v>-0.3166</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.1951</v>
+        <v>-0.1953</v>
       </c>
       <c r="T18" t="n">
         <v>-0.0385</v>
@@ -1712,10 +1712,10 @@
         <v>-0.0127</v>
       </c>
       <c r="M20" t="n">
-        <v>-0.0125</v>
+        <v>-0.0126</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.6083</v>
+        <v>-0.6091</v>
       </c>
       <c r="O20" t="n">
         <v>-0.0001</v>
@@ -1771,7 +1771,7 @@
         <v>-0.2502</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.0331</v>
+        <v>-0.0332</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -1830,34 +1830,34 @@
         <v>0.4279</v>
       </c>
       <c r="K22" t="n">
-        <v>0.3665</v>
+        <v>0.463</v>
       </c>
       <c r="L22" t="n">
-        <v>0.0923</v>
+        <v>0.0924</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0444</v>
+        <v>0.0445</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2217</v>
+        <v>0.222</v>
       </c>
       <c r="O22" t="n">
-        <v>0.3137</v>
+        <v>0.314</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.0626</v>
+        <v>-0.0628</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.1093</v>
+        <v>-0.1095</v>
       </c>
       <c r="R22" t="n">
-        <v>0.2144</v>
+        <v>0.2146</v>
       </c>
       <c r="S22" t="n">
-        <v>0.1061</v>
+        <v>0.1062</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.0685</v>
+        <v>-0.0687</v>
       </c>
     </row>
     <row r="23">
@@ -1892,34 +1892,34 @@
         <v>-0.0219</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.0177</v>
+        <v>-0.0024</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.0083</v>
+        <v>0.0089</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.0046</v>
+        <v>0.0119</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.0032</v>
+        <v>0.013</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.0029</v>
+        <v>0.0132</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.0016</v>
+        <v>0.0142</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.004</v>
+        <v>0.0199</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0269</v>
+        <v>0.0432</v>
       </c>
       <c r="S23" t="n">
-        <v>-0.0021</v>
+        <v>0.0142</v>
       </c>
       <c r="T23" t="n">
-        <v>-0.0079</v>
+        <v>0.0086</v>
       </c>
     </row>
     <row r="24">
@@ -1954,34 +1954,34 @@
         <v>0.099</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0929</v>
+        <v>0.1091</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1985</v>
+        <v>0.1847</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1611</v>
+        <v>0.1472</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0945</v>
+        <v>0.0806</v>
       </c>
       <c r="O24" t="n">
-        <v>-0.0031</v>
+        <v>-0.0325</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.055</v>
+        <v>-0.0552</v>
       </c>
       <c r="Q24" t="n">
+        <v>-0.0553</v>
+      </c>
+      <c r="R24" t="n">
         <v>-0.0555</v>
       </c>
-      <c r="R24" t="n">
-        <v>-0.0559</v>
-      </c>
       <c r="S24" t="n">
-        <v>-0.0434</v>
+        <v>-0.0429</v>
       </c>
       <c r="T24" t="n">
-        <v>-0.0313</v>
+        <v>-0.0307</v>
       </c>
     </row>
     <row r="25">
@@ -2016,34 +2016,34 @@
         <v>0.2519</v>
       </c>
       <c r="K25" t="n">
-        <v>0.3191</v>
+        <v>0.3912</v>
       </c>
       <c r="L25" t="n">
-        <v>0.1792</v>
+        <v>0.251</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1767</v>
+        <v>0.2128</v>
       </c>
       <c r="N25" t="n">
-        <v>0.1729</v>
+        <v>0.2085</v>
       </c>
       <c r="O25" t="n">
-        <v>0.1557</v>
+        <v>0.1906</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1435</v>
+        <v>0.1778</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.1055</v>
+        <v>0.1394</v>
       </c>
       <c r="R25" t="n">
-        <v>0.0364</v>
+        <v>0.0697</v>
       </c>
       <c r="S25" t="n">
-        <v>0.0099</v>
+        <v>0.0098</v>
       </c>
       <c r="T25" t="n">
-        <v>0.0113</v>
+        <v>0.0111</v>
       </c>
     </row>
     <row r="26">
@@ -2078,7 +2078,7 @@
         <v>0.0018</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.0023</v>
+        <v>-0.0041</v>
       </c>
       <c r="L26" t="n">
         <v>0.0063</v>
@@ -2140,7 +2140,7 @@
         <v>183.8</v>
       </c>
       <c r="K27" t="n">
-        <v>175.4</v>
+        <v>175.5</v>
       </c>
       <c r="L27" t="n">
         <v>189.3096</v>
@@ -2326,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="L30" t="n">
         <v>0</v>
@@ -2456,22 +2456,22 @@
         <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="N32" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="O32" t="n">
-        <v>0.0004</v>
+        <v>0.0003</v>
       </c>
       <c r="P32" t="n">
-        <v>0.0014</v>
+        <v>0.0013</v>
       </c>
       <c r="Q32" t="n">
         <v>0.0006</v>
       </c>
       <c r="R32" t="n">
-        <v>0.0006</v>
+        <v>0.0005</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -2512,34 +2512,34 @@
         <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>1.3404</v>
+        <v>1.3749</v>
       </c>
       <c r="L33" t="n">
-        <v>-1.3452</v>
+        <v>-1.3455</v>
       </c>
       <c r="M33" t="n">
-        <v>0.004</v>
+        <v>0.0037</v>
       </c>
       <c r="N33" t="n">
-        <v>0.0081</v>
+        <v>0.0075</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0101</v>
+        <v>0.0094</v>
       </c>
       <c r="P33" t="n">
-        <v>0.0029</v>
+        <v>0.0027</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.0029</v>
+        <v>0.0027</v>
       </c>
       <c r="R33" t="n">
-        <v>0.0094</v>
+        <v>0.0087</v>
       </c>
       <c r="S33" t="n">
-        <v>32.2654</v>
+        <v>32.2647</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.1226</v>
+        <v>-0.1227</v>
       </c>
     </row>
     <row r="34">
@@ -2574,34 +2574,34 @@
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>0.0096</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0002</v>
+        <v>0.0098</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0008</v>
+        <v>0.0102</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0005</v>
+        <v>0.0098</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0002</v>
+        <v>0.0093</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0003</v>
+        <v>0.0092</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.0001</v>
+        <v>0.0088</v>
       </c>
       <c r="R34" t="n">
-        <v>0.0001</v>
+        <v>0.0144</v>
       </c>
       <c r="S34" t="n">
-        <v>-0.1855</v>
+        <v>-0.1656</v>
       </c>
       <c r="T34" t="n">
-        <v>-0.1883</v>
+        <v>-0.1627</v>
       </c>
     </row>
     <row r="35">
@@ -2636,34 +2636,34 @@
         <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="L35" t="n">
+        <v>-0.0348</v>
+      </c>
+      <c r="M35" t="n">
+        <v>-0.0338</v>
+      </c>
+      <c r="N35" t="n">
+        <v>-0.0313</v>
+      </c>
+      <c r="O35" t="n">
+        <v>-0.0321</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.0027</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="R35" t="n">
         <v>-0.0001</v>
       </c>
-      <c r="M35" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0.0019</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0.0019</v>
-      </c>
-      <c r="P35" t="n">
-        <v>0.0013</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>-0.0001</v>
-      </c>
-      <c r="R35" t="n">
-        <v>-0.0014</v>
-      </c>
       <c r="S35" t="n">
-        <v>5.5461</v>
+        <v>5.5475</v>
       </c>
       <c r="T35" t="n">
-        <v>5.5245</v>
+        <v>5.5261</v>
       </c>
     </row>
     <row r="36">
@@ -2698,34 +2698,34 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>-0.0027</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.001</v>
+        <v>-0.0481</v>
       </c>
       <c r="M36" t="n">
-        <v>-0.005</v>
+        <v>-0.094</v>
       </c>
       <c r="N36" t="n">
-        <v>-0.0107</v>
+        <v>-0.1186</v>
       </c>
       <c r="O36" t="n">
-        <v>-0.0107</v>
+        <v>-0.1367</v>
       </c>
       <c r="P36" t="n">
-        <v>-0.0113</v>
+        <v>-0.1546</v>
       </c>
       <c r="Q36" t="n">
-        <v>-0.0094</v>
+        <v>-0.1724</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.0051</v>
+        <v>-0.184</v>
       </c>
       <c r="S36" t="n">
-        <v>-7.4565</v>
+        <v>-7.6475</v>
       </c>
       <c r="T36" t="n">
-        <v>-7.3088</v>
+        <v>-7.4936</v>
       </c>
     </row>
     <row r="37">
@@ -2763,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="M37" t="n">
         <v>0.0005</v>
@@ -2787,7 +2787,7 @@
         <v>0.0035</v>
       </c>
       <c r="T37" t="n">
-        <v>0.0025</v>
+        <v>0.0024</v>
       </c>
     </row>
     <row r="38">
@@ -2825,19 +2825,19 @@
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0005</v>
+        <v>0.0004</v>
       </c>
       <c r="M38" t="n">
-        <v>0.002</v>
+        <v>0.0019</v>
       </c>
       <c r="N38" t="n">
-        <v>0.0013</v>
+        <v>0.0012</v>
       </c>
       <c r="O38" t="n">
         <v>0.001</v>
       </c>
       <c r="P38" t="n">
-        <v>0.0009</v>
+        <v>0.0008</v>
       </c>
       <c r="Q38" t="n">
         <v>0.0005</v>
@@ -2884,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>-0.0006</v>
       </c>
       <c r="L39" t="n">
         <v>0</v>
@@ -2946,34 +2946,34 @@
         <v>-0.0743</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.0437</v>
+        <v>-0.0401</v>
       </c>
       <c r="L40" t="n">
-        <v>-0.0742</v>
+        <v>-0.0706</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0048</v>
+        <v>0.0082</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0063</v>
+        <v>0.0095</v>
       </c>
       <c r="O40" t="n">
-        <v>-0.0237</v>
+        <v>-0.0238</v>
       </c>
       <c r="P40" t="n">
-        <v>0.0046</v>
+        <v>0.0045</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.0038</v>
+        <v>0.0037</v>
       </c>
       <c r="R40" t="n">
-        <v>0.0044</v>
+        <v>0.0043</v>
       </c>
       <c r="S40" t="n">
-        <v>6.6293</v>
+        <v>6.6292</v>
       </c>
       <c r="T40" t="n">
-        <v>6.5085</v>
+        <v>6.5084</v>
       </c>
     </row>
     <row r="41">
@@ -2984,58 +2984,58 @@
         <v>49</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>0.0646</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>0.0296</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.0274</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>0.0173</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>-0.0131</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>-0.0124</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>-0.0118</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>-0.0109</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>-0.0095</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>-0.1412</v>
       </c>
       <c r="M41" t="n">
-        <v>-0.0001</v>
+        <v>-0.1177</v>
       </c>
       <c r="N41" t="n">
-        <v>-0.0001</v>
+        <v>-0.108</v>
       </c>
       <c r="O41" t="n">
-        <v>0</v>
+        <v>-0.0974</v>
       </c>
       <c r="P41" t="n">
-        <v>0</v>
+        <v>-0.0583</v>
       </c>
       <c r="Q41" t="n">
-        <v>0</v>
+        <v>-0.0323</v>
       </c>
       <c r="R41" t="n">
-        <v>0</v>
+        <v>-0.0319</v>
       </c>
       <c r="S41" t="n">
-        <v>0.0052</v>
+        <v>-0.0202</v>
       </c>
       <c r="T41" t="n">
-        <v>0.0037</v>
+        <v>0.0022</v>
       </c>
     </row>
     <row r="42">
@@ -3073,25 +3073,25 @@
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0031</v>
+        <v>0.0023</v>
       </c>
       <c r="M42" t="n">
+        <v>0.0043</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.0034</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.0061</v>
+      </c>
+      <c r="P42" t="n">
         <v>0.0046</v>
       </c>
-      <c r="N42" t="n">
-        <v>0.0036</v>
-      </c>
-      <c r="O42" t="n">
-        <v>0.0066</v>
-      </c>
-      <c r="P42" t="n">
-        <v>0.0049</v>
-      </c>
       <c r="Q42" t="n">
-        <v>0.0021</v>
+        <v>0.002</v>
       </c>
       <c r="R42" t="n">
-        <v>0.0007</v>
+        <v>0.0006</v>
       </c>
       <c r="S42" t="n">
         <v>0.0592</v>
@@ -3135,10 +3135,10 @@
         <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0007</v>
+        <v>0.0005</v>
       </c>
       <c r="M43" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
@@ -3170,58 +3170,58 @@
         <v>49</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>0.0646</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>0.0296</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>0.0274</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>0.0173</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>-0.0131</v>
       </c>
       <c r="H44" t="n">
-        <v>0.2262</v>
+        <v>0.169</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.0471</v>
+        <v>-0.0891</v>
       </c>
       <c r="J44" t="n">
-        <v>0.3108</v>
+        <v>0.2847</v>
       </c>
       <c r="K44" t="n">
-        <v>0.4717</v>
+        <v>0.5251</v>
       </c>
       <c r="L44" t="n">
-        <v>0.4582</v>
+        <v>0.1578</v>
       </c>
       <c r="M44" t="n">
-        <v>0.3454</v>
+        <v>0.1577</v>
       </c>
       <c r="N44" t="n">
-        <v>0.1632</v>
+        <v>0.036</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.0765</v>
+        <v>-0.3273</v>
       </c>
       <c r="P44" t="n">
-        <v>-0.2112</v>
+        <v>-0.3286</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.2118</v>
+        <v>-0.3175</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.7086</v>
+        <v>-0.3933</v>
       </c>
       <c r="S44" t="n">
-        <v>72.1432</v>
+        <v>72.203</v>
       </c>
       <c r="T44" t="n">
-        <v>1.9752</v>
+        <v>1.6735</v>
       </c>
     </row>
     <row r="45">
@@ -3256,34 +3256,34 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>142.5993</v>
+        <v>106.1993</v>
       </c>
       <c r="L45" t="n">
-        <v>541.3327</v>
+        <v>504.6185</v>
       </c>
       <c r="M45" t="n">
-        <v>546.7735</v>
+        <v>509.6903</v>
       </c>
       <c r="N45" t="n">
-        <v>553.0265</v>
+        <v>515.5192</v>
       </c>
       <c r="O45" t="n">
-        <v>559.6347</v>
+        <v>521.6792</v>
       </c>
       <c r="P45" t="n">
-        <v>566.3776</v>
+        <v>527.9648</v>
       </c>
       <c r="Q45" t="n">
-        <v>573.3592</v>
+        <v>534.4729</v>
       </c>
       <c r="R45" t="n">
-        <v>580.4735</v>
+        <v>541.1047</v>
       </c>
       <c r="S45" t="n">
-        <v>587.4184</v>
+        <v>547.5786</v>
       </c>
       <c r="T45" t="n">
-        <v>594.2653</v>
+        <v>553.9611</v>
       </c>
     </row>
     <row r="46">
@@ -3318,19 +3318,19 @@
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>1.3404</v>
+        <v>1.3551</v>
       </c>
       <c r="L46" t="n">
-        <v>-1.3455</v>
+        <v>-1.3457</v>
       </c>
       <c r="M46" t="n">
         <v>0.0012</v>
       </c>
       <c r="N46" t="n">
-        <v>0.0053</v>
+        <v>0.005</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0076</v>
+        <v>0.0071</v>
       </c>
       <c r="P46" t="n">
         <v>0.0003</v>
@@ -3339,10 +3339,10 @@
         <v>-0.0002</v>
       </c>
       <c r="R46" t="n">
-        <v>0.0065</v>
+        <v>0.006</v>
       </c>
       <c r="S46" t="n">
-        <v>6.5549</v>
+        <v>6.5546</v>
       </c>
       <c r="T46" t="n">
         <v>-0.0385</v>
@@ -3448,10 +3448,10 @@
         <v>0.0001</v>
       </c>
       <c r="M48" t="n">
-        <v>0.0003</v>
+        <v>0.0002</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0124</v>
+        <v>0.0116</v>
       </c>
       <c r="O48" t="n">
         <v>0</v>
@@ -3507,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="M49" t="n">
         <v>0</v>
@@ -3566,34 +3566,34 @@
         <v>0</v>
       </c>
       <c r="K50" t="n">
-        <v>-1.3404</v>
+        <v>-1.2439</v>
       </c>
       <c r="L50" t="n">
-        <v>1.3457</v>
+        <v>1.3458</v>
       </c>
       <c r="M50" t="n">
         <v>-0.0009</v>
       </c>
       <c r="N50" t="n">
-        <v>-0.0045</v>
+        <v>-0.0043</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.0064</v>
+        <v>-0.006</v>
       </c>
       <c r="P50" t="n">
-        <v>0.0013</v>
+        <v>0.0011</v>
       </c>
       <c r="Q50" t="n">
-        <v>0.0022</v>
+        <v>0.002</v>
       </c>
       <c r="R50" t="n">
-        <v>-0.0044</v>
+        <v>-0.0042</v>
       </c>
       <c r="S50" t="n">
-        <v>38.1627</v>
+        <v>38.1628</v>
       </c>
       <c r="T50" t="n">
-        <v>-0.0685</v>
+        <v>-0.0687</v>
       </c>
     </row>
     <row r="51">
@@ -3628,34 +3628,34 @@
         <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>0.0153</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>0.0173</v>
       </c>
       <c r="M51" t="n">
-        <v>0.0001</v>
+        <v>0.0166</v>
       </c>
       <c r="N51" t="n">
-        <v>0.0001</v>
+        <v>0.0163</v>
       </c>
       <c r="O51" t="n">
-        <v>0.0001</v>
+        <v>0.0161</v>
       </c>
       <c r="P51" t="n">
-        <v>0</v>
+        <v>0.0158</v>
       </c>
       <c r="Q51" t="n">
-        <v>-0.0001</v>
+        <v>0.0159</v>
       </c>
       <c r="R51" t="n">
-        <v>-0.0005</v>
+        <v>0.0157</v>
       </c>
       <c r="S51" t="n">
-        <v>-0.0613</v>
+        <v>-0.0449</v>
       </c>
       <c r="T51" t="n">
-        <v>-0.0613</v>
+        <v>-0.0449</v>
       </c>
     </row>
     <row r="52">
@@ -3690,34 +3690,34 @@
         <v>0</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>0.0161</v>
       </c>
       <c r="L52" t="n">
-        <v>-0.0011</v>
+        <v>-0.0149</v>
       </c>
       <c r="M52" t="n">
-        <v>-0.0033</v>
+        <v>-0.0172</v>
       </c>
       <c r="N52" t="n">
-        <v>-0.0019</v>
+        <v>-0.0159</v>
       </c>
       <c r="O52" t="n">
-        <v>0.0001</v>
+        <v>-0.0293</v>
       </c>
       <c r="P52" t="n">
-        <v>0.0011</v>
+        <v>0.001</v>
       </c>
       <c r="Q52" t="n">
-        <v>0.0011</v>
+        <v>0.0013</v>
       </c>
       <c r="R52" t="n">
-        <v>0.0011</v>
+        <v>0.0016</v>
       </c>
       <c r="S52" t="n">
-        <v>0.7709</v>
+        <v>0.7714</v>
       </c>
       <c r="T52" t="n">
-        <v>0.7537</v>
+        <v>0.7542</v>
       </c>
     </row>
     <row r="53">
@@ -3752,34 +3752,34 @@
         <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>0.072</v>
       </c>
       <c r="L53" t="n">
-        <v>-0.001</v>
+        <v>0.0709</v>
       </c>
       <c r="M53" t="n">
-        <v>-0.0036</v>
+        <v>0.0325</v>
       </c>
       <c r="N53" t="n">
-        <v>-0.0035</v>
+        <v>0.032</v>
       </c>
       <c r="O53" t="n">
-        <v>-0.0032</v>
+        <v>0.0317</v>
       </c>
       <c r="P53" t="n">
-        <v>-0.0029</v>
+        <v>0.0315</v>
       </c>
       <c r="Q53" t="n">
-        <v>-0.0022</v>
+        <v>0.0317</v>
       </c>
       <c r="R53" t="n">
-        <v>-0.0007</v>
+        <v>0.0325</v>
       </c>
       <c r="S53" t="n">
-        <v>-3.9089</v>
+        <v>-3.9091</v>
       </c>
       <c r="T53" t="n">
-        <v>-3.865</v>
+        <v>-3.8652</v>
       </c>
     </row>
     <row r="54">
@@ -3814,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="K54" t="n">
-        <v>0</v>
+        <v>-0.0018</v>
       </c>
       <c r="L54" t="n">
         <v>0</v>
@@ -3876,7 +3876,7 @@
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L55" t="n">
         <v>0</v>
@@ -4006,7 +4006,7 @@
         <v>0</v>
       </c>
       <c r="M57" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="N57" t="n">
         <v>-0.0001</v>
@@ -4018,7 +4018,7 @@
         <v>-0.0002</v>
       </c>
       <c r="Q57" t="n">
-        <v>-0.0003</v>
+        <v>-0.0002</v>
       </c>
       <c r="R57" t="n">
         <v>-0.0002</v>

</xml_diff>